<commit_message>
Another terrible commit of far too much stuff
</commit_message>
<xml_diff>
--- a/data/raw/API_PNECs.xlsx
+++ b/data/raw/API_PNECs.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/346ebfb30976329f/Projects/Papers/03_Bayesian_Mixture_Toxicity/API_RQ_BN/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/346ebfb30976329f/Projects/Papers/03_Bayesian_Mixture_Toxicity/API_RQ_BN_IEAM_revision/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{E456DB70-8780-4E30-99E5-258EFC1918C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD8E074-AA9B-4A78-A461-3A149883CD8D}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="8_{E456DB70-8780-4E30-99E5-258EFC1918C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F21D535-A956-4AF8-A9CB-A9F8E619A14B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{9F0A2065-8426-49E8-B31C-D12E528CF06C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9F0A2065-8426-49E8-B31C-D12E528CF06C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$4</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,75 +34,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>API_Name</t>
   </si>
   <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>ethinylestradiol</t>
+  </si>
+  <si>
+    <t>estradiol</t>
+  </si>
+  <si>
+    <t>diclofenac</t>
+  </si>
+  <si>
+    <t>ciprofloxacin</t>
+  </si>
+  <si>
+    <t>ibuprofen</t>
+  </si>
+  <si>
+    <t>paracetamol</t>
+  </si>
+  <si>
+    <t>https://www.fass.se/LIF/product?userType=0&amp;nplId=20110119000014&amp;docType=78&amp;scrollPosition=306</t>
+  </si>
+  <si>
+    <t>https://www.aces.su.se/aces/wp-content/uploads/2018/11/Ciprofloxacin-EQS-data-overview-2018.pdf</t>
+  </si>
+  <si>
+    <t>https://health.ec.europa.eu/publications/scheer-scientific-opinion-draft-environmental-quality-standards-priority-substances-under-water-6_en</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>Most_Sensitive_Endpoint</t>
+  </si>
+  <si>
+    <t>https://health.ec.europa.eu/system/files/2022-03/scheer_o_023.pdf</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Value_ugL</t>
+  </si>
+  <si>
+    <t>Value_ngL</t>
+  </si>
+  <si>
+    <t>AA-QS_fw,eco (SSD)</t>
+  </si>
+  <si>
+    <t>AA-QS_fw,eco (deterministic)</t>
+  </si>
+  <si>
+    <t>Danio rerio</t>
+  </si>
+  <si>
+    <t>uncertain</t>
+  </si>
+  <si>
+    <t>https://health.ec.europa.eu/system/files/2022-08/scheer_o_038.pdf</t>
+  </si>
+  <si>
+    <t>Mesocosm /weight of evidence approach</t>
+  </si>
+  <si>
+    <t>Anabaena flos-aquae</t>
+  </si>
+  <si>
+    <t>AA-QS_fw,eco (deterministic &amp; SSD, weight of evidence)</t>
+  </si>
+  <si>
+    <t>Daphnia magna</t>
+  </si>
+  <si>
     <t>PNEC</t>
   </si>
   <si>
-    <t>PNEC_gL</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>ethinylestradiol</t>
-  </si>
-  <si>
-    <t>https://publications.jrc.ec.europa.eu/repository/bitstream/JRC111198/wl_report_jrc_2018_04_26_final_online.pdf</t>
-  </si>
-  <si>
-    <t>estradiol</t>
-  </si>
-  <si>
-    <t>4.00E-4 µg/L</t>
-  </si>
-  <si>
-    <t>17-beta-Estradiol</t>
-  </si>
-  <si>
-    <t>diclofenac</t>
-  </si>
-  <si>
-    <t>5.00E-2 µg/L</t>
-  </si>
-  <si>
-    <t>17-alpha-Ethinylestradiol</t>
-  </si>
-  <si>
-    <t>ciprofloxacin</t>
-  </si>
-  <si>
-    <t>ibuprofen</t>
-  </si>
-  <si>
-    <t>paracetamol</t>
-  </si>
-  <si>
-    <t>1.00E+0 µg/L</t>
-  </si>
-  <si>
-    <t>3.50E-5 µg/L</t>
-  </si>
-  <si>
-    <t>5.00E-3 µg/L</t>
-  </si>
-  <si>
-    <t>https://www.felleskatalogen.no/medisin/nurofen-reckitt-benckiser-585436</t>
-  </si>
-  <si>
-    <t>https://www.felleskatalogen.no/medisin/ciprofloxacin-actavis-547507#egenskap</t>
-  </si>
-  <si>
-    <t>https://www.fass.se/LIF/product?userType=0&amp;nplId=20110119000014&amp;docType=78&amp;scrollPosition=306</t>
-  </si>
-  <si>
-    <t>1.00E+1 µg/L</t>
+    <t>Value_mgL</t>
+  </si>
+  <si>
+    <t>Value_ugL_standard</t>
   </si>
 </sst>
 </file>
@@ -464,137 +482,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B6CBB5-93B2-4F98-B7A4-FB670694F09D}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="105.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="105.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="1">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <f>B2/1000</f>
+        <v>3.2000000000000003E-6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B3">
+        <v>0.18</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <f>B3/1000</f>
+        <v>1.7999999999999998E-4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <f>C4</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C5" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E7" si="0">C5</f>
+        <v>0.04</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1">
-        <v>4.9999999999999998E-8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>4.0000000000000001E-10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.5000000000000002E-11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5.0000000000000001E-9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G9" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E4" xr:uid="{6039041E-2E36-45E7-8678-BC729A34FA7A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E4">
+  <autoFilter ref="A1:F4" xr:uid="{6039041E-2E36-45E7-8678-BC729A34FA7A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
+      <sortCondition ref="C1:C4"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F4">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>